<commit_message>
Clean code y final casos de uso
</commit_message>
<xml_diff>
--- a/Casos de Prueba y Manual/Casos de prueba.xlsx
+++ b/Casos de Prueba y Manual/Casos de prueba.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="55">
   <si>
     <t>ID</t>
   </si>
@@ -51,9 +51,6 @@
     <t xml:space="preserve">Se permite subir fotos de la mascota </t>
   </si>
   <si>
-    <t>Se permite al usuario hacer la publicación de la mascota en adopción en su Facebook</t>
-  </si>
-  <si>
     <t xml:space="preserve">El sistema permite que el usuario pueda editar la información de la mascota </t>
   </si>
   <si>
@@ -75,15 +72,6 @@
     <t xml:space="preserve">El sistema debe permitir registrar adopciones de mascotas </t>
   </si>
   <si>
-    <t>El sistema debe guardar y hacer la conección entre la mascota y el adoptante</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sistema debe permitir registrar fotos del nuevo dueño mostrando la nueva vida de la mascota </t>
-  </si>
-  <si>
-    <t>Sistema debe permitir al usuario hacer la publicación en su usuario de Facebook de las fotos de la adopción</t>
-  </si>
-  <si>
     <t>El sistema debe de permitir al usuario devolver la mascota</t>
   </si>
   <si>
@@ -96,51 +84,18 @@
     <t xml:space="preserve">El sistema debe permitir calificar los adoptantes </t>
   </si>
   <si>
-    <t>Las calificaciones se mostraran en estrellas del 1 al 5</t>
-  </si>
-  <si>
-    <t>El sistema debe permitir escribir comentarios a los adoptantes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">El sistema debe permitir que los que dieron en adopción puedan reportar al adoptante  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Al reportar al adoptante se mete en la lista negra automático </t>
-  </si>
-  <si>
     <t>El sistema debe permitir a la persona hacer un test de recomendación de adopciones</t>
   </si>
   <si>
-    <t xml:space="preserve">Las preguntas del test deben ser parametrizables por el administrador </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Las preguntas del test deben ser modificable por el administrador </t>
-  </si>
-  <si>
-    <t>El sistema debe ejecutar un proveso que consiste en identificar todas las mascotas que no han sido adoptadas en los últimos 2 meses</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Los 2 meses deben de ser parametrizables </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Estas mascotas que no han sido adoptadas en los últimos 2 meses deben de estar en la pantalla principal </t>
-  </si>
-  <si>
     <t>Debe de haber un formulario para el que quiera adoptar</t>
   </si>
   <si>
-    <t xml:space="preserve">El formulario debe de ser parametrizable </t>
-  </si>
-  <si>
     <t xml:space="preserve">El resultado del formulario debe de ser mandado al rescatista para escoger entre todas las solicitudes cual será el más adecuado </t>
   </si>
   <si>
     <t>El sistema debe de permitir hacer consultas de mascotas</t>
   </si>
   <si>
-    <t>Debe de permitir hace consultas por lugar</t>
-  </si>
-  <si>
     <t>Debe de permitir hace consultas por estado</t>
   </si>
   <si>
@@ -165,35 +120,77 @@
     <t xml:space="preserve">Debe de mostrar la cantidad de mascotas que han sido devueltas  </t>
   </si>
   <si>
-    <t xml:space="preserve">El sistema debe mostrar los Top 10 de motivos de devolución de mascotas </t>
-  </si>
-  <si>
-    <t xml:space="preserve">El sistema debe mostrar los Top 10 mejores adoptantes </t>
-  </si>
-  <si>
     <t>El sistema debe permitir mostrar el listado de adoptantes en lista negra</t>
   </si>
   <si>
-    <t xml:space="preserve">*Los valores y mensajes de correos deben de ser parametrizables </t>
-  </si>
-  <si>
     <t xml:space="preserve">El sistema debe de permitir hacer un log out correctamente </t>
   </si>
   <si>
     <t>Se permite hacer consulta de la persona por nombre</t>
   </si>
   <si>
-    <t xml:space="preserve">Se permite hacer consulta de la persona por estado </t>
-  </si>
-  <si>
     <t>Correcto</t>
+  </si>
+  <si>
+    <t>El sistema debe permitir que los que dieron en adopción puedan reportar al adoptante  por medio de calificación</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Al tener una calificación menor de 0 se mete en la lista negra automático </t>
+  </si>
+  <si>
+    <t>El sistema debe guardar y hacer la conección entre la mascota y el adoptante internamente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sistema debe permitir que el nuevo adoptante edite los datos de la mascota adoptada </t>
+  </si>
+  <si>
+    <t>El administriador debe de poder editar las categorías que se utilizan para registrar la mascota</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El administrador debe de poder agregar categorías que se utilizan para registrar la mascota </t>
+  </si>
+  <si>
+    <t>El administrador debe de poder editar las razones de devolución de las mascotas</t>
+  </si>
+  <si>
+    <t>El administrador debe de poder eliminar las razones de devolución de las mascotas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El administrador debe de poder crear nuevas razones de devolución de las mascotasl </t>
+  </si>
+  <si>
+    <t>El formulario debe de ser parametrizable por el dueño que lo puso en adopción</t>
+  </si>
+  <si>
+    <t>Debe de permitir hace consultas por tamaño</t>
+  </si>
+  <si>
+    <t>Debe de permitir hace consultas por color</t>
+  </si>
+  <si>
+    <t>Debe de permitir hace consultas por espacio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Debe de permitir hace consultas por energía </t>
+  </si>
+  <si>
+    <t>El sistema muestra si el usuario esta en lista negra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Si el usuario ingresado es rescatista le aparecen las opciones de registered Pets </t>
+  </si>
+  <si>
+    <t>Si el usuario ingresado no es rescatista le aparecen la opción de adopted Pets</t>
+  </si>
+  <si>
+    <t>Cuando uno escoge el tipo de mascota le aparecen las razas de solamente ese tipo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -217,6 +214,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -235,7 +239,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -253,11 +257,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="25">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -266,6 +279,10 @@
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -274,6 +291,10 @@
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -603,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -637,7 +658,10 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>36</v>
+      </c>
+      <c r="D2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -648,7 +672,10 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>55</v>
+        <v>36</v>
+      </c>
+      <c r="D3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -659,7 +686,10 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>36</v>
+      </c>
+      <c r="D4" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -670,7 +700,10 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
+        <v>36</v>
+      </c>
+      <c r="D5" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -681,7 +714,10 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>55</v>
+        <v>36</v>
+      </c>
+      <c r="D6" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -692,7 +728,10 @@
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>55</v>
+        <v>36</v>
+      </c>
+      <c r="D7" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -703,7 +742,10 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>55</v>
+        <v>36</v>
+      </c>
+      <c r="D8" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -714,7 +756,10 @@
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>55</v>
+        <v>36</v>
+      </c>
+      <c r="D9" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -725,7 +770,10 @@
         <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>55</v>
+        <v>36</v>
+      </c>
+      <c r="D10" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -733,10 +781,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>55</v>
+        <v>36</v>
+      </c>
+      <c r="D11" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -744,10 +795,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>54</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>55</v>
+        <v>36</v>
+      </c>
+      <c r="D12" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -755,10 +809,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>53</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>55</v>
+        <v>36</v>
+      </c>
+      <c r="D13" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -766,10 +823,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>36</v>
+      </c>
+      <c r="D14" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -777,10 +837,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
+        <v>36</v>
+      </c>
+      <c r="D15" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -788,406 +851,503 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="C16" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>36</v>
+      </c>
+      <c r="D16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="C17" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>36</v>
+      </c>
+      <c r="D17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+        <v>36</v>
+      </c>
+      <c r="D18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+        <v>36</v>
+      </c>
+      <c r="D19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+        <v>36</v>
+      </c>
+      <c r="D20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+        <v>36</v>
+      </c>
+      <c r="D21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="C22" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
+        <v>36</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="C23" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
+        <v>36</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="C24" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
+        <v>36</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C25" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
+        <v>36</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="C26" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
+        <v>36</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="C27" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
+        <v>36</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="C28" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
+        <v>36</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="C29" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
+        <v>36</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="C30" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
+        <v>36</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="C31" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
+        <v>36</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="C32" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
+        <v>36</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="C33" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
+        <v>36</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C34" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
+        <v>36</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="C35" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
+        <v>36</v>
+      </c>
+      <c r="D35" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="C36" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
+        <v>36</v>
+      </c>
+      <c r="D36" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="C37" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
+        <v>36</v>
+      </c>
+      <c r="D37" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="C38" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
+        <v>36</v>
+      </c>
+      <c r="D38" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="C39" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
+        <v>36</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C40" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
+        <v>36</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="C41" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
+        <v>36</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="C42" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
+        <v>36</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="C43" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
+        <v>36</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C44" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
+        <v>36</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C45" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
+        <v>36</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="C46" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
+        <v>36</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="C47" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
+        <v>36</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="C48" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
+        <v>36</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C49" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
+        <v>36</v>
+      </c>
+      <c r="D49" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C50" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
+        <v>36</v>
+      </c>
+      <c r="D50" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>51</v>
-      </c>
-      <c r="C51" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="A52">
-        <v>51</v>
-      </c>
-      <c r="B52" t="s">
-        <v>52</v>
-      </c>
-      <c r="C52" t="s">
-        <v>55</v>
+        <v>54</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>